<commit_message>
Identify edit permission instead of incorrect copyright status
</commit_message>
<xml_diff>
--- a/Bibles/index.xlsx
+++ b/Bibles/index.xlsx
@@ -35,7 +35,7 @@
     <t>ZefaniaBibleName</t>
   </si>
   <si>
-    <t>ZefaniaBibleWithoutCopyright</t>
+    <t>ZefaniaBibleFreeToEditLicenseType</t>
   </si>
   <si>
     <t>ZefaniaBibleStatus</t>
@@ -113,7 +113,7 @@
     <t>1933/1953 Afrikaans Bybel</t>
   </si>
   <si>
-    <t>False</t>
+    <t>None</t>
   </si>
   <si>
     <t>v</t>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>Bulgarian New Testament from 1914, known as 'Tsarigrad Edition'</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t>2.0.1.22</t>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t>Chamorro: Y Santa Biblia (1908)</t>
+  </si>
+  <si>
+    <t>PublicDomain</t>
   </si>
   <si>
     <t>Chamorro Y Santa Biblia (1908)</t>
@@ -6621,7 +6621,7 @@
     <col min="5" max="5" width="10.882190159389" customWidth="1"/>
     <col min="6" max="6" width="25.3329881940569" customWidth="1"/>
     <col min="7" max="7" width="61.2845284598214" customWidth="1"/>
-    <col min="8" max="8" width="28.7121734619141" customWidth="1"/>
+    <col min="8" max="8" width="33.0653163364955" customWidth="1"/>
     <col min="9" max="9" width="18.1449312482561" customWidth="1"/>
     <col min="10" max="10" width="19.3838631766183" customWidth="1"/>
     <col min="11" max="11" width="20.107171194894" customWidth="1"/>
@@ -7130,13 +7130,13 @@
         <v>95</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>36</v>
@@ -7148,25 +7148,25 @@
         <v>95</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>67</v>
       </c>
       <c r="P7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="S7" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>40</v>
@@ -7186,16 +7186,16 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>30</v>
@@ -7204,7 +7204,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>33</v>
@@ -7213,7 +7213,7 @@
         <v>34</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>36</v>
@@ -7222,28 +7222,28 @@
         <v>37</v>
       </c>
       <c r="M8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>67</v>
       </c>
       <c r="P8" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q8" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="R8" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>111</v>
       </c>
       <c r="S8" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>40</v>
@@ -7263,16 +7263,16 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>30</v>
@@ -7281,7 +7281,7 @@
         <v>31</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>33</v>
@@ -7293,63 +7293,63 @@
         <v>35</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>37</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N9" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="P9" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="Q9" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S9" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T9" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="U9" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="U9" s="0" t="s">
+      <c r="V9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="X9" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="V9" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="X9" s="0" t="s">
+      <c r="Y9" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="Y9" s="0" t="s">
+      <c r="Z9" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z9" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>30</v>
@@ -7358,7 +7358,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>33</v>
@@ -7370,63 +7370,63 @@
         <v>35</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>37</v>
       </c>
       <c r="M10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="N10" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="O10" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="P10" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="Q10" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="U10" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="U10" s="0" t="s">
+      <c r="V10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="X10" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="V10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="X10" s="0" t="s">
+      <c r="Y10" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="Y10" s="0" t="s">
+      <c r="Z10" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z10" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>137</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>30</v>
@@ -7435,16 +7435,16 @@
         <v>31</v>
       </c>
       <c r="G11" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>36</v>
@@ -7462,10 +7462,10 @@
         <v>67</v>
       </c>
       <c r="P11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="Q11" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="R11" s="0" t="s">
         <v>141</v>
@@ -7678,7 +7678,7 @@
         <v>35</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>37</v>
@@ -7746,7 +7746,7 @@
         <v>173</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>34</v>
@@ -7823,7 +7823,7 @@
         <v>186</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>34</v>
@@ -7951,7 +7951,7 @@
         <v>205</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18">
@@ -7986,7 +7986,7 @@
         <v>174</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>37</v>
@@ -8063,7 +8063,7 @@
         <v>35</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>37</v>
@@ -8294,7 +8294,7 @@
         <v>35</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>37</v>
@@ -8522,7 +8522,7 @@
         <v>34</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>36</v>
@@ -8540,7 +8540,7 @@
         <v>67</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q25" s="0" t="s">
         <v>265</v>
@@ -8599,10 +8599,10 @@
         <v>34</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>37</v>
@@ -8617,7 +8617,7 @@
         <v>67</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q26" s="0" t="s">
         <v>226</v>
@@ -8721,7 +8721,7 @@
         <v>205</v>
       </c>
       <c r="Z27" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
@@ -8875,7 +8875,7 @@
         <v>204</v>
       </c>
       <c r="Z29" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
@@ -8949,7 +8949,7 @@
         <v>47</v>
       </c>
       <c r="Y30" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z30" s="0" t="s">
         <v>306</v>
@@ -9026,7 +9026,7 @@
         <v>149</v>
       </c>
       <c r="Y31" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z31" s="0" t="s">
         <v>306</v>
@@ -9061,7 +9061,7 @@
         <v>34</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>36</v>
@@ -9334,10 +9334,10 @@
         <v>47</v>
       </c>
       <c r="Y35" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z35" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z35" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="36">
@@ -9363,7 +9363,7 @@
         <v>352</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>34</v>
@@ -9488,7 +9488,7 @@
         <v>149</v>
       </c>
       <c r="Y37" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z37" s="0" t="s">
         <v>306</v>
@@ -9517,7 +9517,7 @@
         <v>367</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>34</v>
@@ -9568,7 +9568,7 @@
         <v>204</v>
       </c>
       <c r="Z38" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39">
@@ -9642,7 +9642,7 @@
         <v>47</v>
       </c>
       <c r="Y39" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z39" s="0" t="s">
         <v>306</v>
@@ -9831,7 +9831,7 @@
         <v>34</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K42" s="0" t="s">
         <v>36</v>
@@ -9911,7 +9911,7 @@
         <v>35</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L43" s="0" t="s">
         <v>37</v>
@@ -9953,7 +9953,7 @@
         <v>204</v>
       </c>
       <c r="Z43" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44">
@@ -9985,7 +9985,7 @@
         <v>34</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K44" s="0" t="s">
         <v>36</v>
@@ -10003,7 +10003,7 @@
         <v>67</v>
       </c>
       <c r="P44" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q44" s="0" t="s">
         <v>420</v>
@@ -10287,7 +10287,7 @@
         <v>449</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>34</v>
@@ -10373,7 +10373,7 @@
         <v>35</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L49" s="0" t="s">
         <v>37</v>
@@ -10415,7 +10415,7 @@
         <v>204</v>
       </c>
       <c r="Z49" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50">
@@ -10450,7 +10450,7 @@
         <v>35</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L50" s="0" t="s">
         <v>37</v>
@@ -10486,13 +10486,13 @@
         <v>40</v>
       </c>
       <c r="X50" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y50" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="Y50" s="0" t="s">
+      <c r="Z50" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z50" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="51">
@@ -10566,7 +10566,7 @@
         <v>149</v>
       </c>
       <c r="Y51" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z51" s="0" t="s">
         <v>306</v>
@@ -10595,7 +10595,7 @@
         <v>478</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>34</v>
@@ -10720,7 +10720,7 @@
         <v>47</v>
       </c>
       <c r="Y53" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z53" s="0" t="s">
         <v>489</v>
@@ -10758,7 +10758,7 @@
         <v>35</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L54" s="0" t="s">
         <v>37</v>
@@ -10835,7 +10835,7 @@
         <v>35</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L55" s="0" t="s">
         <v>37</v>
@@ -10874,7 +10874,7 @@
         <v>504</v>
       </c>
       <c r="Y55" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z55" s="0" t="s">
         <v>48</v>
@@ -10954,7 +10954,7 @@
         <v>204</v>
       </c>
       <c r="Z56" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57">
@@ -11031,7 +11031,7 @@
         <v>204</v>
       </c>
       <c r="Z57" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58">
@@ -11066,7 +11066,7 @@
         <v>35</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L58" s="0" t="s">
         <v>37</v>
@@ -11108,7 +11108,7 @@
         <v>204</v>
       </c>
       <c r="Z58" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59">
@@ -11143,7 +11143,7 @@
         <v>35</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L59" s="0" t="s">
         <v>37</v>
@@ -11179,13 +11179,13 @@
         <v>40</v>
       </c>
       <c r="X59" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y59" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="Y59" s="0" t="s">
+      <c r="Z59" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z59" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="60">
@@ -11294,7 +11294,7 @@
         <v>34</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K61" s="0" t="s">
         <v>36</v>
@@ -11365,7 +11365,7 @@
         <v>553</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>34</v>
@@ -11442,7 +11442,7 @@
         <v>560</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I63" s="0" t="s">
         <v>34</v>
@@ -11519,7 +11519,7 @@
         <v>546</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>34</v>
@@ -11596,7 +11596,7 @@
         <v>576</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I65" s="0" t="s">
         <v>34</v>
@@ -11647,7 +11647,7 @@
         <v>205</v>
       </c>
       <c r="Z65" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66">
@@ -11673,7 +11673,7 @@
         <v>584</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I66" s="0" t="s">
         <v>34</v>
@@ -11724,7 +11724,7 @@
         <v>205</v>
       </c>
       <c r="Z66" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67">
@@ -11750,7 +11750,7 @@
         <v>592</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>34</v>
@@ -11801,7 +11801,7 @@
         <v>205</v>
       </c>
       <c r="Z67" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68">
@@ -11827,7 +11827,7 @@
         <v>546</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>34</v>
@@ -11878,7 +11878,7 @@
         <v>205</v>
       </c>
       <c r="Z68" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69">
@@ -11904,7 +11904,7 @@
         <v>605</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I69" s="0" t="s">
         <v>34</v>
@@ -11955,7 +11955,7 @@
         <v>205</v>
       </c>
       <c r="Z69" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70">
@@ -12029,10 +12029,10 @@
         <v>47</v>
       </c>
       <c r="Y70" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z70" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z70" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="71">
@@ -12067,7 +12067,7 @@
         <v>35</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L71" s="0" t="s">
         <v>37</v>
@@ -12109,7 +12109,7 @@
         <v>204</v>
       </c>
       <c r="Z71" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72">
@@ -12218,7 +12218,7 @@
         <v>34</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K73" s="0" t="s">
         <v>36</v>
@@ -12289,7 +12289,7 @@
         <v>642</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I74" s="0" t="s">
         <v>34</v>
@@ -12298,7 +12298,7 @@
         <v>35</v>
       </c>
       <c r="K74" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L74" s="0" t="s">
         <v>37</v>
@@ -12340,7 +12340,7 @@
         <v>204</v>
       </c>
       <c r="Z74" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75">
@@ -12366,7 +12366,7 @@
         <v>649</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="I75" s="0" t="s">
         <v>34</v>
@@ -12375,7 +12375,7 @@
         <v>35</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L75" s="0" t="s">
         <v>37</v>
@@ -12417,7 +12417,7 @@
         <v>204</v>
       </c>
       <c r="Z75" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76">
@@ -12529,7 +12529,7 @@
         <v>35</v>
       </c>
       <c r="K77" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L77" s="0" t="s">
         <v>37</v>
@@ -12565,13 +12565,13 @@
         <v>40</v>
       </c>
       <c r="X77" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y77" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="Y77" s="0" t="s">
+      <c r="Z77" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z77" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="78">
@@ -12879,7 +12879,7 @@
         <v>204</v>
       </c>
       <c r="Z81" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82">
@@ -12973,7 +12973,7 @@
         <v>34</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K83" s="0" t="s">
         <v>36</v>
@@ -13130,7 +13130,7 @@
         <v>35</v>
       </c>
       <c r="K85" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L85" s="0" t="s">
         <v>37</v>
@@ -13169,10 +13169,10 @@
         <v>47</v>
       </c>
       <c r="Y85" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z85" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z85" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="86">
@@ -13272,7 +13272,7 @@
         <v>204</v>
       </c>
       <c r="Z87" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88">
@@ -13307,7 +13307,7 @@
         <v>35</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L88" s="0" t="s">
         <v>37</v>
@@ -13346,7 +13346,7 @@
         <v>40</v>
       </c>
       <c r="Y88" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z88" s="0" t="s">
         <v>758</v>
@@ -13423,7 +13423,7 @@
         <v>47</v>
       </c>
       <c r="Y89" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z89" s="0" t="s">
         <v>306</v>
@@ -13577,7 +13577,7 @@
         <v>781</v>
       </c>
       <c r="Y91" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z91" s="0" t="s">
         <v>48</v>
@@ -13692,7 +13692,7 @@
         <v>35</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L93" s="0" t="s">
         <v>37</v>
@@ -13731,7 +13731,7 @@
         <v>47</v>
       </c>
       <c r="Y93" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z93" s="0" t="s">
         <v>306</v>
@@ -13760,7 +13760,7 @@
         <v>800</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I94" s="0" t="s">
         <v>34</v>
@@ -13837,7 +13837,7 @@
         <v>807</v>
       </c>
       <c r="H95" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I95" s="0" t="s">
         <v>34</v>
@@ -13923,7 +13923,7 @@
         <v>35</v>
       </c>
       <c r="K96" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L96" s="0" t="s">
         <v>37</v>
@@ -13959,10 +13959,10 @@
         <v>40</v>
       </c>
       <c r="X96" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y96" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="Y96" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="Z96" s="0" t="s">
         <v>306</v>
@@ -14039,7 +14039,7 @@
         <v>149</v>
       </c>
       <c r="Y97" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z97" s="0" t="s">
         <v>48</v>
@@ -14145,13 +14145,13 @@
         <v>834</v>
       </c>
       <c r="H99" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I99" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K99" s="0" t="s">
         <v>36</v>
@@ -14228,7 +14228,7 @@
         <v>34</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K100" s="0" t="s">
         <v>36</v>
@@ -14299,7 +14299,7 @@
         <v>854</v>
       </c>
       <c r="H101" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I101" s="0" t="s">
         <v>34</v>
@@ -14376,7 +14376,7 @@
         <v>860</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I102" s="0" t="s">
         <v>34</v>
@@ -14427,7 +14427,7 @@
         <v>205</v>
       </c>
       <c r="Z102" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103">
@@ -14459,7 +14459,7 @@
         <v>34</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K103" s="0" t="s">
         <v>36</v>
@@ -14536,7 +14536,7 @@
         <v>34</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K104" s="0" t="s">
         <v>36</v>
@@ -14581,7 +14581,7 @@
         <v>40</v>
       </c>
       <c r="Z104" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="105">
@@ -14607,13 +14607,13 @@
         <v>883</v>
       </c>
       <c r="H105" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I105" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K105" s="0" t="s">
         <v>884</v>
@@ -14684,13 +14684,13 @@
         <v>893</v>
       </c>
       <c r="H106" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I106" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K106" s="0" t="s">
         <v>36</v>
@@ -14708,7 +14708,7 @@
         <v>67</v>
       </c>
       <c r="P106" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q106" s="0" t="s">
         <v>895</v>
@@ -14809,7 +14809,7 @@
         <v>204</v>
       </c>
       <c r="Y107" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z107" s="0" t="s">
         <v>48</v>
@@ -14844,7 +14844,7 @@
         <v>34</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K108" s="0" t="s">
         <v>36</v>
@@ -14889,7 +14889,7 @@
         <v>40</v>
       </c>
       <c r="Z108" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109">
@@ -14924,7 +14924,7 @@
         <v>35</v>
       </c>
       <c r="K109" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L109" s="0" t="s">
         <v>37</v>
@@ -14963,7 +14963,7 @@
         <v>204</v>
       </c>
       <c r="Y109" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z109" s="0" t="s">
         <v>48</v>
@@ -14998,10 +14998,10 @@
         <v>34</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K110" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L110" s="0" t="s">
         <v>37</v>
@@ -15043,7 +15043,7 @@
         <v>40</v>
       </c>
       <c r="Z110" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111">
@@ -15069,7 +15069,7 @@
         <v>931</v>
       </c>
       <c r="H111" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I111" s="0" t="s">
         <v>34</v>
@@ -15117,7 +15117,7 @@
         <v>47</v>
       </c>
       <c r="Y111" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z111" s="0" t="s">
         <v>48</v>
@@ -15194,7 +15194,7 @@
         <v>47</v>
       </c>
       <c r="Y112" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z112" s="0" t="s">
         <v>48</v>
@@ -15223,16 +15223,16 @@
         <v>947</v>
       </c>
       <c r="H113" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I113" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K113" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L113" s="0" t="s">
         <v>37</v>
@@ -15274,7 +15274,7 @@
         <v>40</v>
       </c>
       <c r="Z113" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114">
@@ -15306,7 +15306,7 @@
         <v>34</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K114" s="0" t="s">
         <v>36</v>
@@ -15377,7 +15377,7 @@
         <v>965</v>
       </c>
       <c r="H115" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I115" s="0" t="s">
         <v>34</v>
@@ -15386,7 +15386,7 @@
         <v>35</v>
       </c>
       <c r="K115" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L115" s="0" t="s">
         <v>37</v>
@@ -15425,7 +15425,7 @@
         <v>47</v>
       </c>
       <c r="Y115" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z115" s="0" t="s">
         <v>48</v>
@@ -15463,7 +15463,7 @@
         <v>174</v>
       </c>
       <c r="K116" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L116" s="0" t="s">
         <v>37</v>
@@ -15505,7 +15505,7 @@
         <v>205</v>
       </c>
       <c r="Z116" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="117">
@@ -15531,7 +15531,7 @@
         <v>982</v>
       </c>
       <c r="H117" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I117" s="0" t="s">
         <v>34</v>
@@ -15614,7 +15614,7 @@
         <v>34</v>
       </c>
       <c r="J118" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K118" s="0" t="s">
         <v>36</v>
@@ -15771,7 +15771,7 @@
         <v>35</v>
       </c>
       <c r="K120" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L120" s="0" t="s">
         <v>37</v>
@@ -15810,10 +15810,10 @@
         <v>1008</v>
       </c>
       <c r="Y120" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z120" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z120" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="121">
@@ -15839,7 +15839,7 @@
         <v>1016</v>
       </c>
       <c r="H121" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I121" s="0" t="s">
         <v>34</v>
@@ -15925,7 +15925,7 @@
         <v>35</v>
       </c>
       <c r="K122" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L122" s="0" t="s">
         <v>37</v>
@@ -15993,7 +15993,7 @@
         <v>1035</v>
       </c>
       <c r="H123" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I123" s="0" t="s">
         <v>34</v>
@@ -16044,7 +16044,7 @@
         <v>444</v>
       </c>
       <c r="Z123" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124">
@@ -16070,7 +16070,7 @@
         <v>1044</v>
       </c>
       <c r="H124" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I124" s="0" t="s">
         <v>34</v>
@@ -16118,10 +16118,10 @@
         <v>1048</v>
       </c>
       <c r="Y124" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z124" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z124" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="125">
@@ -16147,7 +16147,7 @@
         <v>1044</v>
       </c>
       <c r="H125" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I125" s="0" t="s">
         <v>34</v>
@@ -16195,10 +16195,10 @@
         <v>1048</v>
       </c>
       <c r="Y125" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z125" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z125" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="126">
@@ -16272,7 +16272,7 @@
         <v>1048</v>
       </c>
       <c r="Y126" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z126" s="0" t="s">
         <v>48</v>
@@ -16455,7 +16455,7 @@
         <v>1084</v>
       </c>
       <c r="H129" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I129" s="0" t="s">
         <v>34</v>
@@ -16464,7 +16464,7 @@
         <v>35</v>
       </c>
       <c r="K129" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L129" s="0" t="s">
         <v>37</v>
@@ -16609,7 +16609,7 @@
         <v>1100</v>
       </c>
       <c r="H131" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I131" s="0" t="s">
         <v>34</v>
@@ -16686,7 +16686,7 @@
         <v>1110</v>
       </c>
       <c r="H132" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I132" s="0" t="s">
         <v>34</v>
@@ -16734,10 +16734,10 @@
         <v>1048</v>
       </c>
       <c r="Y132" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z132" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z132" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="133">
@@ -16763,7 +16763,7 @@
         <v>1117</v>
       </c>
       <c r="H133" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I133" s="0" t="s">
         <v>34</v>
@@ -16840,7 +16840,7 @@
         <v>1117</v>
       </c>
       <c r="H134" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I134" s="0" t="s">
         <v>34</v>
@@ -16917,7 +16917,7 @@
         <v>1134</v>
       </c>
       <c r="H135" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I135" s="0" t="s">
         <v>34</v>
@@ -16965,10 +16965,10 @@
         <v>1048</v>
       </c>
       <c r="Y135" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z135" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z135" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="136">
@@ -16994,7 +16994,7 @@
         <v>1140</v>
       </c>
       <c r="H136" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I136" s="0" t="s">
         <v>34</v>
@@ -17042,7 +17042,7 @@
         <v>1048</v>
       </c>
       <c r="Y136" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z136" s="0" t="s">
         <v>48</v>
@@ -17071,7 +17071,7 @@
         <v>1147</v>
       </c>
       <c r="H137" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I137" s="0" t="s">
         <v>34</v>
@@ -17119,7 +17119,7 @@
         <v>1048</v>
       </c>
       <c r="Y137" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z137" s="0" t="s">
         <v>48</v>
@@ -17154,7 +17154,7 @@
         <v>34</v>
       </c>
       <c r="J138" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K138" s="0" t="s">
         <v>36</v>
@@ -17276,7 +17276,7 @@
         <v>204</v>
       </c>
       <c r="Z139" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="140">
@@ -17308,7 +17308,7 @@
         <v>34</v>
       </c>
       <c r="J140" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K140" s="0" t="s">
         <v>36</v>
@@ -17385,7 +17385,7 @@
         <v>34</v>
       </c>
       <c r="J141" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K141" s="0" t="s">
         <v>36</v>
@@ -17584,7 +17584,7 @@
         <v>40</v>
       </c>
       <c r="Z143" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="144">
@@ -17661,7 +17661,7 @@
         <v>40</v>
       </c>
       <c r="Z144" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="145">
@@ -17770,7 +17770,7 @@
         <v>34</v>
       </c>
       <c r="J146" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K146" s="0" t="s">
         <v>301</v>
@@ -17841,7 +17841,7 @@
         <v>1221</v>
       </c>
       <c r="H147" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I147" s="0" t="s">
         <v>34</v>
@@ -17966,10 +17966,10 @@
         <v>1232</v>
       </c>
       <c r="Y148" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z148" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z148" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="149">
@@ -18004,7 +18004,7 @@
         <v>35</v>
       </c>
       <c r="K149" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L149" s="0" t="s">
         <v>37</v>
@@ -18046,7 +18046,7 @@
         <v>204</v>
       </c>
       <c r="Z149" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="150">
@@ -18158,7 +18158,7 @@
         <v>35</v>
       </c>
       <c r="K151" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L151" s="0" t="s">
         <v>37</v>
@@ -18232,7 +18232,7 @@
         <v>34</v>
       </c>
       <c r="J152" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K152" s="0" t="s">
         <v>345</v>
@@ -18380,7 +18380,7 @@
         <v>1277</v>
       </c>
       <c r="H154" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I154" s="0" t="s">
         <v>34</v>
@@ -18688,7 +18688,7 @@
         <v>1309</v>
       </c>
       <c r="H158" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I158" s="0" t="s">
         <v>34</v>
@@ -18774,7 +18774,7 @@
         <v>35</v>
       </c>
       <c r="K159" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L159" s="0" t="s">
         <v>37</v>
@@ -18816,7 +18816,7 @@
         <v>204</v>
       </c>
       <c r="Z159" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="160">
@@ -18851,7 +18851,7 @@
         <v>35</v>
       </c>
       <c r="K160" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L160" s="0" t="s">
         <v>37</v>
@@ -18893,7 +18893,7 @@
         <v>204</v>
       </c>
       <c r="Z160" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="161">
@@ -18919,7 +18919,7 @@
         <v>1331</v>
       </c>
       <c r="H161" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I161" s="0" t="s">
         <v>34</v>
@@ -19150,7 +19150,7 @@
         <v>1354</v>
       </c>
       <c r="H164" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I164" s="0" t="s">
         <v>34</v>
@@ -19198,7 +19198,7 @@
         <v>1357</v>
       </c>
       <c r="Y164" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z164" s="0" t="s">
         <v>48</v>
@@ -19227,7 +19227,7 @@
         <v>1362</v>
       </c>
       <c r="H165" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I165" s="0" t="s">
         <v>34</v>
@@ -19275,7 +19275,7 @@
         <v>1357</v>
       </c>
       <c r="Y165" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z165" s="0" t="s">
         <v>48</v>
@@ -19429,7 +19429,7 @@
         <v>1357</v>
       </c>
       <c r="Y167" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z167" s="0" t="s">
         <v>48</v>
@@ -19467,7 +19467,7 @@
         <v>35</v>
       </c>
       <c r="K168" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L168" s="0" t="s">
         <v>37</v>
@@ -19660,7 +19660,7 @@
         <v>40</v>
       </c>
       <c r="Y170" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z170" s="0" t="s">
         <v>306</v>
@@ -19775,7 +19775,7 @@
         <v>35</v>
       </c>
       <c r="K172" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L172" s="0" t="s">
         <v>37</v>
@@ -19814,10 +19814,10 @@
         <v>47</v>
       </c>
       <c r="Y172" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z172" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z172" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="173">
@@ -19929,7 +19929,7 @@
         <v>35</v>
       </c>
       <c r="K174" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L174" s="0" t="s">
         <v>37</v>
@@ -19971,7 +19971,7 @@
         <v>204</v>
       </c>
       <c r="Z174" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="175">
@@ -20048,7 +20048,7 @@
         <v>204</v>
       </c>
       <c r="Z175" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="176">
@@ -20160,7 +20160,7 @@
         <v>35</v>
       </c>
       <c r="K177" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L177" s="0" t="s">
         <v>37</v>
@@ -20202,7 +20202,7 @@
         <v>204</v>
       </c>
       <c r="Z177" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="178">
@@ -20391,7 +20391,7 @@
         <v>35</v>
       </c>
       <c r="K180" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L180" s="0" t="s">
         <v>37</v>
@@ -20767,7 +20767,7 @@
         <v>1512</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I185" s="0" t="s">
         <v>34</v>
@@ -20992,7 +20992,7 @@
         <v>1537</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>34</v>
@@ -21155,7 +21155,7 @@
         <v>35</v>
       </c>
       <c r="K190" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L190" s="0" t="s">
         <v>37</v>
@@ -21271,10 +21271,10 @@
         <v>40</v>
       </c>
       <c r="Y191" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z191" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z191" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="192">
@@ -21348,10 +21348,10 @@
         <v>40</v>
       </c>
       <c r="Y192" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z192" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="Z192" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="193">
@@ -21386,7 +21386,7 @@
         <v>35</v>
       </c>
       <c r="K193" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L193" s="0" t="s">
         <v>37</v>
@@ -21608,7 +21608,7 @@
         <v>1589</v>
       </c>
       <c r="H196" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I196" s="0" t="s">
         <v>34</v>
@@ -21617,7 +21617,7 @@
         <v>174</v>
       </c>
       <c r="K196" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L196" s="0" t="s">
         <v>37</v>
@@ -21810,7 +21810,7 @@
         <v>1616</v>
       </c>
       <c r="Y198" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z198" s="0" t="s">
         <v>48</v>
@@ -21839,7 +21839,7 @@
         <v>1621</v>
       </c>
       <c r="H199" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I199" s="0" t="s">
         <v>34</v>
@@ -22153,10 +22153,10 @@
         <v>34</v>
       </c>
       <c r="J203" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K203" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L203" s="0" t="s">
         <v>37</v>
@@ -22233,7 +22233,7 @@
         <v>35</v>
       </c>
       <c r="K204" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L204" s="0" t="s">
         <v>37</v>
@@ -22455,13 +22455,13 @@
         <v>1681</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I207" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J207" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K207" s="0" t="s">
         <v>36</v>
@@ -22541,7 +22541,7 @@
         <v>35</v>
       </c>
       <c r="K208" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L208" s="0" t="s">
         <v>37</v>
@@ -22609,7 +22609,7 @@
         <v>1698</v>
       </c>
       <c r="H209" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I209" s="0" t="s">
         <v>34</v>
@@ -22840,7 +22840,7 @@
         <v>1725</v>
       </c>
       <c r="H212" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I212" s="0" t="s">
         <v>34</v>
@@ -22891,7 +22891,7 @@
         <v>205</v>
       </c>
       <c r="Z212" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="213">
@@ -22962,10 +22962,10 @@
         <v>40</v>
       </c>
       <c r="X213" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y213" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="Y213" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="Z213" s="0" t="s">
         <v>758</v>
@@ -22994,7 +22994,7 @@
         <v>1746</v>
       </c>
       <c r="H214" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I214" s="0" t="s">
         <v>34</v>
@@ -23045,7 +23045,7 @@
         <v>205</v>
       </c>
       <c r="Z214" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="215">
@@ -23199,7 +23199,7 @@
         <v>40</v>
       </c>
       <c r="Z216" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="217">
@@ -23353,7 +23353,7 @@
         <v>40</v>
       </c>
       <c r="Z218" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="219">
@@ -23542,7 +23542,7 @@
         <v>35</v>
       </c>
       <c r="K221" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L221" s="0" t="s">
         <v>37</v>
@@ -23847,7 +23847,7 @@
         <v>34</v>
       </c>
       <c r="J225" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K225" s="0" t="s">
         <v>36</v>
@@ -23865,7 +23865,7 @@
         <v>67</v>
       </c>
       <c r="P225" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q225" s="0" t="s">
         <v>1830</v>
@@ -23918,7 +23918,7 @@
         <v>1837</v>
       </c>
       <c r="H226" s="0" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I226" s="0" t="s">
         <v>34</v>
@@ -24081,7 +24081,7 @@
         <v>35</v>
       </c>
       <c r="K228" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L228" s="0" t="s">
         <v>37</v>
@@ -24232,7 +24232,7 @@
         <v>34</v>
       </c>
       <c r="J230" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K230" s="0" t="s">
         <v>36</v>
@@ -24354,7 +24354,7 @@
         <v>40</v>
       </c>
       <c r="Z231" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="232">
@@ -24481,7 +24481,7 @@
         <v>67</v>
       </c>
       <c r="P233" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q233" s="0" t="s">
         <v>1896</v>
@@ -24662,7 +24662,7 @@
         <v>205</v>
       </c>
       <c r="Z235" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="236">
@@ -24816,7 +24816,7 @@
         <v>205</v>
       </c>
       <c r="Z237" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="238">
@@ -24893,7 +24893,7 @@
         <v>205</v>
       </c>
       <c r="Z238" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="239">
@@ -24970,7 +24970,7 @@
         <v>205</v>
       </c>
       <c r="Z239" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>